<commit_message>
Records: MCS: The Finale
</commit_message>
<xml_diff>
--- a/ygo-records.xlsx
+++ b/ygo-records.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lance\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\c4lance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="457">
   <si>
     <t>5-Round Swiss</t>
   </si>
@@ -1954,6 +1954,21 @@
   </si>
   <si>
     <t>Starter Deck Joey</t>
+  </si>
+  <si>
+    <t>Estrada, Jovanni</t>
+  </si>
+  <si>
+    <t>Casandag, Charles</t>
+  </si>
+  <si>
+    <t>2W-1L-0D</t>
+  </si>
+  <si>
+    <t>Demo Deck 2015 Tournament</t>
+  </si>
+  <si>
+    <t>Starter Deck 2002 Tournament</t>
   </si>
 </sst>
 </file>
@@ -2113,7 +2128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2226,9 +2241,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2238,8 +2250,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2545,37 +2564,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>359</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="34" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="M1" s="36" t="s">
         <v>28</v>
       </c>
       <c r="N1" s="19" t="s">
@@ -2587,19 +2606,19 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
       <c r="N2" s="21" t="s">
         <v>268</v>
       </c>
@@ -2609,19 +2628,19 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="21" t="s">
         <v>365</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
       <c r="H3" s="19">
         <f>SUM(H6:H1508)</f>
         <v>345</v>
@@ -6612,6 +6631,9 @@
       <c r="A176" s="15" t="s">
         <v>176</v>
       </c>
+      <c r="B176" s="38" t="s">
+        <v>455</v>
+      </c>
       <c r="N176" s="32" t="s">
         <v>179</v>
       </c>
@@ -13734,8 +13756,14 @@
       <c r="A510" s="15" t="s">
         <v>176</v>
       </c>
+      <c r="B510" s="38" t="s">
+        <v>456</v>
+      </c>
       <c r="N510" s="32" t="s">
         <v>447</v>
+      </c>
+      <c r="O510" s="2" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="511" spans="1:15" x14ac:dyDescent="0.25">
@@ -13745,6 +13773,9 @@
       <c r="B511" s="1" t="s">
         <v>440</v>
       </c>
+      <c r="C511" s="2" t="s">
+        <v>452</v>
+      </c>
       <c r="D511" s="2" t="s">
         <v>450</v>
       </c>
@@ -13762,6 +13793,9 @@
       <c r="B512" s="1" t="s">
         <v>440</v>
       </c>
+      <c r="C512" s="2" t="s">
+        <v>453</v>
+      </c>
       <c r="D512" s="2" t="s">
         <v>451</v>
       </c>
@@ -13797,17 +13831,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:D2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -19813,7 +19847,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="27">
-        <f t="shared" ref="F3:F65" si="0">SUM(C3:E3)</f>
+        <f t="shared" ref="F3" si="0">SUM(C3:E3)</f>
         <v>4</v>
       </c>
       <c r="G3" s="25">
@@ -19829,7 +19863,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="27">
-        <f t="shared" ref="J3:J65" si="1">SUM(G3:I3)</f>
+        <f t="shared" ref="J3" si="1">SUM(G3:I3)</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>